<commit_message>
Made a few colour choices for the product items. Now to impliment the color picking screen in the product making screen. This will be done in a stack panel with different colour buttons matching new profiles made
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -1,30 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4666D16B-2186-4C64-89D8-9D53F97E54EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Product Sheet" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Product Sheet" sheetId="2" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>FUCK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>YEAH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>NO</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="1" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -40,38 +56,32 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -359,16 +369,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:A3"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A4" sqref="A4"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>

</xml_diff>

<commit_message>
4 themes added notes added for code to be done for the button theme select
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -1,46 +1,57 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4666D16B-2186-4C64-89D8-9D53F97E54EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Product Sheet" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Product Sheet" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
-    <x:t>FUCK</x:t>
-  </x:si>
-  <x:si>
-    <x:t>YEAH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>NO</x:t>
+    <x:t>PRODUCT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PRICE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>THEME</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BUTTON TYPE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1" x14ac:knownFonts="1">
+  <x:fonts count="2">
     <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -56,32 +67,45 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+  <x:cellStyleXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <x:cellXfs count="2">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -369,31 +393,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A3"/>
+  <x:dimension ref="A1:D1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A4" sqref="A4"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="1" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="5.996339" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.424911" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="13.282054" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="0" t="s">
+    <x:row r="1" spans="1:4" s="1" customFormat="1">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:4">
       <x:c r="A2" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
test colors working. now to code saving string to excel to save theme and foreground choice of item
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520547D7-3143-4302-ADA7-719A5FF978CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Product Sheet" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Product Sheet" sheetId="2" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
@@ -25,25 +32,30 @@
     <x:t>THEME</x:t>
   </x:si>
   <x:si>
+    <x:t>FOREGROUND</x:t>
+  </x:si>
+  <x:si>
     <x:t>BUTTON TYPE</x:t>
   </x:si>
   <x:si>
-    <x:t>test</x:t>
-  </x:si>
-  <x:si>
-    <x:t>20</x:t>
+    <x:t>theme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>foreground</x:t>
+  </x:si>
+  <x:si>
+    <x:t>button type</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2">
+  <x:fonts count="2" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -51,7 +63,6 @@
     </x:font>
     <x:font>
       <x:b/>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -67,45 +78,36 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -393,23 +395,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D1"/>
+  <x:dimension ref="A1:E1"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="F24" sqref="F24"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="5.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="7.424911" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="13.282054" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="9.710938" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.425781" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="13.855469" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="13.285156" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" s="1" customFormat="1">
+    <x:row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -422,13 +427,19 @@
       <x:c r="D1" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
+      <x:c r="E1" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
-      <x:c r="A2" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
+    <x:row r="28" spans="1:5">
+      <x:c r="C28" s="0" t="s">
         <x:v>5</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E28" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
color for theme saves. now need to adjust so that cancel saves old data if existing edited
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520547D7-3143-4302-ADA7-719A5FF978CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85633E81-D117-4D64-9C40-7E1918975897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -36,15 +36,6 @@
   </x:si>
   <x:si>
     <x:t>BUTTON TYPE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>theme</x:t>
-  </x:si>
-  <x:si>
-    <x:t>foreground</x:t>
-  </x:si>
-  <x:si>
-    <x:t>button type</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -402,16 +393,16 @@
   <x:dimension ref="A1:E1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="F24" sqref="F24"/>
+      <x:selection activeCell="D15" sqref="D15"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.710938" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="7.425781" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="13.855469" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="13.285156" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="9.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="5.996339" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.424911" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="13.853482" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="13.282054" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -431,17 +422,6 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="28" spans="1:5">
-      <x:c r="C28" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="E28" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
added more themes and foreground for item selection. discovered clicking window throughs error when shecking for button
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -36,6 +36,42 @@
   </x:si>
   <x:si>
     <x:t>BUTTON TYPE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pear</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>btnOrchidItemTheme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DarkGreen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>wet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>btnDefaultItemTheme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Green</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test</x:t>
+  </x:si>
+  <x:si>
+    <x:t>32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>btnLimeGreenItemTheme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Red</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -400,7 +436,7 @@
   <x:cols>
     <x:col min="1" max="1" width="9.710625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="5.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="7.424911" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="24.139196" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.853482" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.282054" style="0" customWidth="1"/>
   </x:cols>
@@ -420,6 +456,48 @@
       </x:c>
       <x:c r="E1" s="1" t="s">
         <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5">
+      <x:c r="A11" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:5">
+      <x:c r="A21" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C21" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:5">
+      <x:c r="A34" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B34" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C34" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D34" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
themes work. border around text boxes now change
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -50,16 +50,16 @@
     <x:t>DarkGreen</x:t>
   </x:si>
   <x:si>
-    <x:t>wet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11</x:t>
-  </x:si>
-  <x:si>
     <x:t>btnDefaultItemTheme</x:t>
   </x:si>
   <x:si>
-    <x:t>Green</x:t>
+    <x:t>Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>btnBrightBlueItemTheme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yellow</x:t>
   </x:si>
   <x:si>
     <x:t>test</x:t>
@@ -473,17 +473,29 @@
       </x:c>
     </x:row>
     <x:row r="21" spans="1:5">
-      <x:c r="A21" s="0" t="s">
+      <x:c r="C21" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="B21" s="0" t="s">
+      <x:c r="D21" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="C21" s="0" t="s">
+    </x:row>
+    <x:row r="22" spans="1:5">
+      <x:c r="C22" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D21" s="0" t="s">
+      <x:c r="D22" s="0" t="s">
         <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:5">
+      <x:c r="C28" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:5">
+      <x:c r="C29" s="0" t="s">
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:5">

</xml_diff>

<commit_message>
button theme for till map now customiszes and transfers between run
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -1,22 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85633E81-D117-4D64-9C40-7E1918975897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Product Sheet" sheetId="2" r:id="rId1"/>
+    <x:sheet name="Product Sheet" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="0"/>
+  <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
@@ -38,51 +31,52 @@
     <x:t>BUTTON TYPE</x:t>
   </x:si>
   <x:si>
-    <x:t>pear</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>btnOrchidItemTheme</x:t>
+    <x:t>ORANGE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>btnDefaultItemTheme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Black</x:t>
+  </x:si>
+  <x:si>
+    <x:t>PIE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22</x:t>
+  </x:si>
+  <x:si>
+    <x:t>btnLimeGreenItemTheme</x:t>
   </x:si>
   <x:si>
     <x:t>DarkGreen</x:t>
   </x:si>
   <x:si>
-    <x:t>btnDefaultItemTheme</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>btnBrightBlueItemTheme</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Yellow</x:t>
-  </x:si>
-  <x:si>
-    <x:t>test</x:t>
-  </x:si>
-  <x:si>
-    <x:t>32</x:t>
-  </x:si>
-  <x:si>
-    <x:t>btnLimeGreenItemTheme</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Red</x:t>
+    <x:t>GRAVY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>POOP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Green</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
+  <x:fonts count="2">
     <x:font>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -90,6 +84,7 @@
     </x:font>
     <x:font>
       <x:b/>
+      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -105,36 +100,45 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
-  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <x:extLst>
-    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </x:ext>
-    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </x:ext>
-  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -422,26 +426,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:E1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D15" sqref="D15"/>
-    </x:sheetView>
+    <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="5.996339" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.139196" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="24.139196" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.853482" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.282054" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:5" s="1" customFormat="1">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -458,58 +460,74 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s">
+    <x:row r="22" spans="1:5">
+      <x:c r="A22" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
+      <x:c r="B22" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C11" s="0" t="s">
+      <x:c r="C22" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D11" s="0" t="s">
+      <x:c r="D22" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:5">
-      <x:c r="C21" s="0" t="s">
+    <x:row r="23" spans="1:5">
+      <x:c r="A23" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D21" s="0" t="s">
+      <x:c r="B23" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
     </x:row>
-    <x:row r="22" spans="1:5">
-      <x:c r="C22" s="0" t="s">
+    <x:row r="27" spans="1:5">
+      <x:c r="A27" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:5">
+      <x:c r="A33" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:5">
-      <x:c r="C28" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:5">
-      <x:c r="C29" s="0" t="s">
-        <x:v>9</x:v>
+      <x:c r="D33" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:5">
       <x:c r="A34" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B34" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C34" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D34" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
delete button added and is enabled for editing product else diabled
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5F0492-4C14-4FEE-9FB7-77B85C6EB5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Product Sheet" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Product Sheet" sheetId="2" r:id="rId1"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
@@ -30,53 +37,16 @@
   <x:si>
     <x:t>BUTTON TYPE</x:t>
   </x:si>
-  <x:si>
-    <x:t>ORANGE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>btnDefaultItemTheme</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Black</x:t>
-  </x:si>
-  <x:si>
-    <x:t>PIE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>btnLimeGreenItemTheme</x:t>
-  </x:si>
-  <x:si>
-    <x:t>DarkGreen</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GRAVY</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>POOP</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Green</x:t>
-  </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2">
+  <x:fonts count="2" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -84,7 +54,6 @@
     </x:font>
     <x:font>
       <x:b/>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -100,45 +69,36 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
   <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -426,24 +386,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
   <x:dimension ref="A1:E1"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="D34" sqref="D34"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="9.710625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.139196" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="24.139196" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="5.996339" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.424911" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.853482" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.282054" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" s="1" customFormat="1">
+    <x:row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -460,76 +422,6 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:5">
-      <x:c r="A22" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B22" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="C22" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D22" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="23" spans="1:5">
-      <x:c r="A23" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B23" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="C23" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D23" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:5">
-      <x:c r="A27" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:5">
-      <x:c r="A33" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B33" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="C33" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="D33" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="34" spans="1:5">
-      <x:c r="A34" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B34" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="C34" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D34" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Default Them finished just not for sale list as code is not started and will be added in future. Theming will be moved to the property window script or a seperate script
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -36,6 +36,9 @@
   </x:si>
   <x:si>
     <x:t>BUTTON TYPE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Green</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -422,6 +425,11 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
+    <x:row r="34" spans="1:5">
+      <x:c r="D34" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Started on property window now changes from 2 themes and saves file to remember selected theme
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -36,9 +36,6 @@
   </x:si>
   <x:si>
     <x:t>BUTTON TYPE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Green</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -425,11 +422,6 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="34" spans="1:5">
-      <x:c r="D34" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Cleared some un needed lines
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cpljy\source\repos\Projects\NewTillSystem\Resources\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5F0492-4C14-4FEE-9FB7-77B85C6EB5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5A0D80-DDB7-4D2A-961A-8884F0325020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -392,8 +392,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:E1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="D34" sqref="D34"/>
+    <x:sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <x:selection activeCell="G26" sqref="G26"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed product scroll to uniform grid added more product themes and foreground colors
</commit_message>
<xml_diff>
--- a/Resources/XLSX/ProductDataBase.xlsx
+++ b/Resources/XLSX/ProductDataBase.xlsx
@@ -36,6 +36,12 @@
   </x:si>
   <x:si>
     <x:t>BUTTON TYPE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>btnDarkYellowItemTheme</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Red</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -400,7 +406,7 @@
   <x:cols>
     <x:col min="1" max="1" width="9.710625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="5.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="7.424911" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="24.424911" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="13.853482" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="13.282054" style="0" customWidth="1"/>
   </x:cols>
@@ -420,6 +426,14 @@
       </x:c>
       <x:c r="E1" s="1" t="s">
         <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:5">
+      <x:c r="C28" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>6</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>